<commit_message>
correct pe values in september
</commit_message>
<xml_diff>
--- a/lai/valuationquan/CNIESG300index/CNIESG300indexmodel1.xlsx
+++ b/lai/valuationquan/CNIESG300index/CNIESG300indexmodel1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="15600" windowHeight="7620"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="15600" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model1&amp;2" sheetId="5" r:id="rId1"/>
@@ -1649,7 +1649,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1695,451 +1694,451 @@
             <c:numRef>
               <c:f>'model1&amp;2'!时间</c:f>
               <c:numCache>
-                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="148"/>
                 <c:pt idx="0">
-                  <c:v>40451</c:v>
+                  <c:v>1.2300899999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40480</c:v>
+                  <c:v>1.3965399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40512</c:v>
+                  <c:v>1.31427</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40543</c:v>
+                  <c:v>1.29017</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40574</c:v>
+                  <c:v>1.2746999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40602</c:v>
+                  <c:v>1.3761099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40633</c:v>
+                  <c:v>1.3503900000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40662</c:v>
+                  <c:v>1.3469</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40694</c:v>
+                  <c:v>1.27504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40724</c:v>
+                  <c:v>1.3109200000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40753</c:v>
+                  <c:v>1.2869000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40786</c:v>
+                  <c:v>1.2162500000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40816</c:v>
+                  <c:v>1.1052</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40847</c:v>
+                  <c:v>1.1468800000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40877</c:v>
+                  <c:v>1.07321</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40907</c:v>
+                  <c:v>0.99402000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40939</c:v>
+                  <c:v>1.0423</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40968</c:v>
+                  <c:v>1.1305099999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40998</c:v>
+                  <c:v>1.0494400000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41026</c:v>
+                  <c:v>1.1058599999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41060</c:v>
+                  <c:v>1.14459</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41089</c:v>
+                  <c:v>1.0780399999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41121</c:v>
+                  <c:v>1.0063800000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41152</c:v>
+                  <c:v>0.95391999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41180</c:v>
+                  <c:v>0.97826999999999997</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41213</c:v>
+                  <c:v>0.97197</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41243</c:v>
+                  <c:v>0.91870000000000007</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41274</c:v>
+                  <c:v>1.06653</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41305</c:v>
+                  <c:v>1.1200399999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41333</c:v>
+                  <c:v>1.1328399999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41362</c:v>
+                  <c:v>1.0812299999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41390</c:v>
+                  <c:v>1.0785899999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41425</c:v>
+                  <c:v>1.1670399999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41453</c:v>
+                  <c:v>1.0075000000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41486</c:v>
+                  <c:v>1.0311600000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41516</c:v>
+                  <c:v>1.1031</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41547</c:v>
+                  <c:v>1.1687700000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41578</c:v>
+                  <c:v>1.1723299999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41607</c:v>
+                  <c:v>1.2098100000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41639</c:v>
+                  <c:v>1.1735899999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41669</c:v>
+                  <c:v>1.1339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41698</c:v>
+                  <c:v>1.12253</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41729</c:v>
+                  <c:v>1.0989899999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41759</c:v>
+                  <c:v>1.08745</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41789</c:v>
+                  <c:v>1.0986300000000002</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41820</c:v>
+                  <c:v>1.1062000000000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41851</c:v>
+                  <c:v>1.2045899999999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41880</c:v>
+                  <c:v>1.2067399999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41912</c:v>
+                  <c:v>1.27871</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41943</c:v>
+                  <c:v>1.2983800000000001</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41971</c:v>
+                  <c:v>1.41004</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42004</c:v>
+                  <c:v>1.6953900000000002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42034</c:v>
+                  <c:v>1.7145299999999999</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42062</c:v>
+                  <c:v>1.78149</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42094</c:v>
+                  <c:v>2.0250699999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42124</c:v>
+                  <c:v>2.4119800000000002</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42153</c:v>
+                  <c:v>2.5110399999999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42185</c:v>
+                  <c:v>2.3950300000000002</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42216</c:v>
+                  <c:v>2.05552</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42247</c:v>
+                  <c:v>1.8248599999999999</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42277</c:v>
+                  <c:v>1.7126700000000001</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42307</c:v>
+                  <c:v>1.91326</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42338</c:v>
+                  <c:v>1.94798</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42369</c:v>
+                  <c:v>2.09022</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42398</c:v>
+                  <c:v>1.6191</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>42429</c:v>
+                  <c:v>1.56416</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>42460</c:v>
+                  <c:v>1.7538099999999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>42489</c:v>
+                  <c:v>1.73098</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>42521</c:v>
+                  <c:v>1.7421500000000001</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>42551</c:v>
+                  <c:v>1.75274</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>42580</c:v>
+                  <c:v>1.8355599999999999</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>42613</c:v>
+                  <c:v>1.9024799999999999</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>42643</c:v>
+                  <c:v>1.8773900000000001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>42674</c:v>
+                  <c:v>1.9152199999999999</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>42704</c:v>
+                  <c:v>2.0240299999999998</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>42734</c:v>
+                  <c:v>1.9521400000000002</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>42761</c:v>
+                  <c:v>2.0017999999999998</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>42794</c:v>
+                  <c:v>2.08507</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>42825</c:v>
+                  <c:v>2.1146199999999999</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>42853</c:v>
+                  <c:v>2.10263</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>42886</c:v>
+                  <c:v>2.0933999999999999</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>42916</c:v>
+                  <c:v>2.2407399999999997</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>42947</c:v>
+                  <c:v>2.2731599999999998</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>42978</c:v>
+                  <c:v>2.3099499999999997</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>43007</c:v>
+                  <c:v>2.33961</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>43039</c:v>
+                  <c:v>2.4434499999999999</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>43069</c:v>
+                  <c:v>2.42692</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>43098</c:v>
+                  <c:v>2.4915799999999999</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>43131</c:v>
+                  <c:v>2.6026100000000003</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>43159</c:v>
+                  <c:v>2.4634099999999997</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>43189</c:v>
+                  <c:v>2.3982399999999999</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>43217</c:v>
+                  <c:v>2.3119000000000001</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>43251</c:v>
+                  <c:v>2.3675700000000002</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>43280</c:v>
+                  <c:v>2.1851400000000001</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>43312</c:v>
+                  <c:v>2.1775900000000004</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>43343</c:v>
+                  <c:v>2.04325</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>43371</c:v>
+                  <c:v>2.10771</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>43404</c:v>
+                  <c:v>1.88317</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>43434</c:v>
+                  <c:v>1.9444000000000001</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>43462</c:v>
+                  <c:v>1.8736900000000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>43496</c:v>
+                  <c:v>1.9604600000000001</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>43524</c:v>
+                  <c:v>2.2494399999999999</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>43553</c:v>
+                  <c:v>2.4353899999999999</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>43585</c:v>
+                  <c:v>2.42089</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>43616</c:v>
+                  <c:v>2.2623000000000002</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>43644</c:v>
+                  <c:v>2.3454800000000002</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>43677</c:v>
+                  <c:v>2.3299000000000003</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>43707</c:v>
+                  <c:v>2.24383</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>43738</c:v>
+                  <c:v>2.2523499999999999</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>43769</c:v>
+                  <c:v>2.25983</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>43798</c:v>
+                  <c:v>2.2531300000000001</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>43830</c:v>
+                  <c:v>2.4450100000000003</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>43853</c:v>
+                  <c:v>2.3811999999999998</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>43889</c:v>
+                  <c:v>2.3709600000000002</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>43921</c:v>
+                  <c:v>2.1931400000000001</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>43951</c:v>
+                  <c:v>2.2996099999999999</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>43980</c:v>
+                  <c:v>2.3069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>44012</c:v>
+                  <c:v>2.4672199999999997</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>44043</c:v>
+                  <c:v>2.7463200000000003</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>44074</c:v>
+                  <c:v>2.8232600000000003</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>44104</c:v>
+                  <c:v>2.7159299999999997</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>44134</c:v>
+                  <c:v>2.8166100000000003</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>44165</c:v>
+                  <c:v>2.9742600000000001</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>44196</c:v>
+                  <c:v>3.1853200000000004</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>44225</c:v>
+                  <c:v>3.2828000000000004</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>44253</c:v>
+                  <c:v>3.2778700000000001</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>44286</c:v>
+                  <c:v>3.1244299999999998</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>44316</c:v>
+                  <c:v>3.1956700000000002</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>44347</c:v>
+                  <c:v>3.3188599999999999</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>44377</c:v>
+                  <c:v>3.2336</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>44407</c:v>
+                  <c:v>2.9186799999999997</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>44439</c:v>
+                  <c:v>2.91865</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>44469</c:v>
+                  <c:v>2.9991300000000001</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>44498</c:v>
+                  <c:v>3.0190700000000001</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>44530</c:v>
+                  <c:v>2.96435</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>44561</c:v>
+                  <c:v>3.07491</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>44589</c:v>
+                  <c:v>2.8309000000000002</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>44620</c:v>
+                  <c:v>2.8623000000000003</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>44651</c:v>
+                  <c:v>2.6462500000000002</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>44680</c:v>
+                  <c:v>2.5422700195312502</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>44712</c:v>
+                  <c:v>2.5905100097656248</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>44742</c:v>
+                  <c:v>2.8271101074218752</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>44771</c:v>
+                  <c:v>2.6160200195312502</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>44804</c:v>
+                  <c:v>2.5657299804687499</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>44834</c:v>
+                  <c:v>2.4191298828124999</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>44865</c:v>
+                  <c:v>2.1911298828125001</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>44895</c:v>
+                  <c:v>2.4362099609375001</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>44925</c:v>
+                  <c:v>2.4624399414062501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2154,445 +2153,445 @@
                   <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4000</c:v>
+                  <c:v>4270.6306042647284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6000</c:v>
+                  <c:v>6019.0482795100788</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>7908.6759332370966</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10000</c:v>
+                  <c:v>9813.8456266207759</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12000</c:v>
+                  <c:v>12594.595673687232</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14000</c:v>
+                  <c:v>14359.198066862755</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16000</c:v>
+                  <c:v>16322.087601550247</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18000</c:v>
+                  <c:v>17451.269266820571</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20000</c:v>
+                  <c:v>19942.353108342035</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22000</c:v>
+                  <c:v>21576.949177009552</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24000</c:v>
+                  <c:v>22392.388248145049</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26000</c:v>
+                  <c:v>22347.845830914623</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28000</c:v>
+                  <c:v>25190.641898805072</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30000</c:v>
+                  <c:v>25572.51743182947</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32000</c:v>
+                  <c:v>25685.572979740344</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34000</c:v>
+                  <c:v>28933.132851233735</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36000</c:v>
+                  <c:v>33381.74807603209</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>38000</c:v>
+                  <c:v>32987.909616819947</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40000</c:v>
+                  <c:v>36761.405824874695</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42000</c:v>
+                  <c:v>40048.882763725363</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44000</c:v>
+                  <c:v>39720.316947209474</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>46000</c:v>
+                  <c:v>39080.008691080729</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>48000</c:v>
+                  <c:v>39042.86839026583</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>50000</c:v>
+                  <c:v>42039.486393141306</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52000</c:v>
+                  <c:v>43768.754627599286</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>54000</c:v>
+                  <c:v>43369.954706807272</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>56000</c:v>
+                  <c:v>52348.707732068309</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>58000</c:v>
+                  <c:v>56975.149886290856</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>60000</c:v>
+                  <c:v>59626.271202087191</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>62000</c:v>
+                  <c:v>58909.813576350352</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>64000</c:v>
+                  <c:v>60765.975625274667</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>66000</c:v>
+                  <c:v>67749.102248046562</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>68000</c:v>
+                  <c:v>60487.473021410515</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>70000</c:v>
+                  <c:v>63907.953033010097</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>72000</c:v>
+                  <c:v>70366.560951465755</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>74000</c:v>
+                  <c:v>76555.63905651767</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>76000</c:v>
+                  <c:v>78788.822723998164</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>78000</c:v>
+                  <c:v>83307.742376054724</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>80000</c:v>
+                  <c:v>82813.626416639017</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>82000</c:v>
+                  <c:v>82019.983432432651</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>84000</c:v>
+                  <c:v>83190.380954504973</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>86000</c:v>
+                  <c:v>83445.838209394322</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>88000</c:v>
+                  <c:v>84569.610970805807</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>90000</c:v>
+                  <c:v>87439.065429083086</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>92000</c:v>
+                  <c:v>90041.555553418075</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>94000</c:v>
+                  <c:v>100050.2236522255</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>96000</c:v>
+                  <c:v>102228.79725889026</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>98000</c:v>
+                  <c:v>110325.72496388252</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>100000</c:v>
+                  <c:v>114022.8314305869</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>102000</c:v>
+                  <c:v>125828.73521648881</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>104000</c:v>
+                  <c:v>153292.71467382699</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>106000</c:v>
+                  <c:v>157023.30324569365</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>108000</c:v>
+                  <c:v>165155.75959544061</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>110000</c:v>
+                  <c:v>189737.21664670523</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>112000</c:v>
+                  <c:v>227988.4210459491</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>114000</c:v>
+                  <c:v>239351.90374017198</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>116000</c:v>
+                  <c:v>230293.85036272786</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>118000</c:v>
+                  <c:v>199648.30306826817</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>120000</c:v>
+                  <c:v>179244.7859116719</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>122000</c:v>
+                  <c:v>170225.05150386505</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>124000</c:v>
+                  <c:v>192162.01722473378</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>126000</c:v>
+                  <c:v>197649.18846023903</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>128000</c:v>
+                  <c:v>214081.38004669495</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>130000</c:v>
+                  <c:v>167829.03351494283</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>132000</c:v>
+                  <c:v>164134.18631507194</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>134000</c:v>
+                  <c:v>186034.99469442785</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>136000</c:v>
+                  <c:v>185613.30766511807</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>138000</c:v>
+                  <c:v>188811.06884469232</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>140000</c:v>
+                  <c:v>191958.79390801364</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>142000</c:v>
+                  <c:v>203029.179311132</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>144000</c:v>
+                  <c:v>212431.12350227855</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>146000</c:v>
+                  <c:v>211629.57137627876</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>148000</c:v>
+                  <c:v>217893.97391659516</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>150000</c:v>
+                  <c:v>232273.25321707482</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>152000</c:v>
+                  <c:v>226023.31414810085</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>154000</c:v>
+                  <c:v>233773.064565896</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>156000</c:v>
+                  <c:v>245497.45415846378</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>158000</c:v>
+                  <c:v>250976.68975745208</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>160000</c:v>
+                  <c:v>251553.63951192721</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>162000</c:v>
+                  <c:v>252449.38432071661</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>164000</c:v>
+                  <c:v>272217.55680844683</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>166000</c:v>
+                  <c:v>278156.11870841286</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>168000</c:v>
+                  <c:v>284657.94154854841</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>170000</c:v>
+                  <c:v>290312.97933998541</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>172000</c:v>
+                  <c:v>305198.0754776597</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>174000</c:v>
+                  <c:v>305133.40290910058</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>176000</c:v>
+                  <c:v>315263.01815480401</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>178000</c:v>
+                  <c:v>331311.795599529</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>180000</c:v>
+                  <c:v>315591.66006348841</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>182000</c:v>
+                  <c:v>309242.62012034556</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>184000</c:v>
+                  <c:v>300109.45253862289</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>186000</c:v>
+                  <c:v>309336.01650022384</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>188000</c:v>
+                  <c:v>287500.53561047785</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>190000</c:v>
+                  <c:v>288507.17635484249</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>192000</c:v>
+                  <c:v>272708.57603452983</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>194000</c:v>
+                  <c:v>283311.9259971804</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>196000</c:v>
+                  <c:v>255129.94656765409</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>198000</c:v>
+                  <c:v>265425.32437652821</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>200000</c:v>
+                  <c:v>257772.87391023306</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>202000</c:v>
+                  <c:v>271710.25537098217</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>204000</c:v>
+                  <c:v>313761.48293854605</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>206000</c:v>
+                  <c:v>341698.58183979383</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>208000</c:v>
+                  <c:v>341664.15226725023</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>210000</c:v>
+                  <c:v>321282.08703171159</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>212000</c:v>
+                  <c:v>335094.9518150285</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>214000</c:v>
+                  <c:v>334869.06229592022</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>216000</c:v>
+                  <c:v>324498.4969532832</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>218000</c:v>
+                  <c:v>327730.64341448661</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>220000</c:v>
+                  <c:v>330819.02897301014</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>222000</c:v>
+                  <c:v>331838.20851566637</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>224000</c:v>
+                  <c:v>362098.05834678403</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>226000</c:v>
+                  <c:v>354648.00411260565</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>228000</c:v>
+                  <c:v>355122.89258811681</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>230000</c:v>
+                  <c:v>330488.97520443297</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>232000</c:v>
+                  <c:v>348533.16809226322</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>234000</c:v>
+                  <c:v>351653.21023514908</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>236000</c:v>
+                  <c:v>378075.35039287584</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>238000</c:v>
+                  <c:v>422844.47122306196</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>240000</c:v>
+                  <c:v>436690.74318550713</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>242000</c:v>
+                  <c:v>422089.3612844068</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>244000</c:v>
+                  <c:v>439736.28771259688</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>246000</c:v>
+                  <c:v>466349.00504225586</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>248000</c:v>
+                  <c:v>501442.15123802173</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>250000</c:v>
+                  <c:v>518787.73061550414</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>252000</c:v>
+                  <c:v>520008.63243348437</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>254000</c:v>
+                  <c:v>497666.56744597905</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>256000</c:v>
+                  <c:v>511013.84239368205</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>258000</c:v>
+                  <c:v>532712.93374055997</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>260000</c:v>
+                  <c:v>521027.78138983715</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>262000</c:v>
+                  <c:v>472284.93474359531</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>264000</c:v>
+                  <c:v>474280.08030664356</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>266000</c:v>
+                  <c:v>489358.06528705527</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>268000</c:v>
+                  <c:v>494611.60875526897</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>270000</c:v>
+                  <c:v>487646.87881158153</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>272000</c:v>
+                  <c:v>507834.42040464858</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>274000</c:v>
+                  <c:v>469535.13459695398</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>276000</c:v>
+                  <c:v>476743.16145284584</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>278000</c:v>
+                  <c:v>442757.9886785429</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>280000</c:v>
+                  <c:v>427360.55192268913</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>282000</c:v>
+                  <c:v>437469.78842900984</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>284000</c:v>
+                  <c:v>479425.39341558446</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>286000</c:v>
+                  <c:v>445628.43306111766</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>288000</c:v>
+                  <c:v>439061.72824284952</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>290000</c:v>
+                  <c:v>415974.71880401362</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>292000</c:v>
+                  <c:v>378769.61594403378</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>294000</c:v>
+                  <c:v>423135.37791693263</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>296000</c:v>
+                  <c:v>429691.15630892606</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2634,451 +2633,451 @@
             <c:numRef>
               <c:f>'model1&amp;2'!时间</c:f>
               <c:numCache>
-                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="148"/>
                 <c:pt idx="0">
-                  <c:v>40451</c:v>
+                  <c:v>1.2300899999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40480</c:v>
+                  <c:v>1.3965399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40512</c:v>
+                  <c:v>1.31427</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40543</c:v>
+                  <c:v>1.29017</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40574</c:v>
+                  <c:v>1.2746999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40602</c:v>
+                  <c:v>1.3761099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40633</c:v>
+                  <c:v>1.3503900000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40662</c:v>
+                  <c:v>1.3469</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40694</c:v>
+                  <c:v>1.27504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40724</c:v>
+                  <c:v>1.3109200000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40753</c:v>
+                  <c:v>1.2869000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40786</c:v>
+                  <c:v>1.2162500000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40816</c:v>
+                  <c:v>1.1052</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40847</c:v>
+                  <c:v>1.1468800000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40877</c:v>
+                  <c:v>1.07321</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40907</c:v>
+                  <c:v>0.99402000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40939</c:v>
+                  <c:v>1.0423</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40968</c:v>
+                  <c:v>1.1305099999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40998</c:v>
+                  <c:v>1.0494400000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41026</c:v>
+                  <c:v>1.1058599999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41060</c:v>
+                  <c:v>1.14459</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41089</c:v>
+                  <c:v>1.0780399999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41121</c:v>
+                  <c:v>1.0063800000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41152</c:v>
+                  <c:v>0.95391999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41180</c:v>
+                  <c:v>0.97826999999999997</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41213</c:v>
+                  <c:v>0.97197</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41243</c:v>
+                  <c:v>0.91870000000000007</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41274</c:v>
+                  <c:v>1.06653</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41305</c:v>
+                  <c:v>1.1200399999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41333</c:v>
+                  <c:v>1.1328399999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41362</c:v>
+                  <c:v>1.0812299999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41390</c:v>
+                  <c:v>1.0785899999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41425</c:v>
+                  <c:v>1.1670399999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41453</c:v>
+                  <c:v>1.0075000000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41486</c:v>
+                  <c:v>1.0311600000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41516</c:v>
+                  <c:v>1.1031</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41547</c:v>
+                  <c:v>1.1687700000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41578</c:v>
+                  <c:v>1.1723299999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41607</c:v>
+                  <c:v>1.2098100000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41639</c:v>
+                  <c:v>1.1735899999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41669</c:v>
+                  <c:v>1.1339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41698</c:v>
+                  <c:v>1.12253</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41729</c:v>
+                  <c:v>1.0989899999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41759</c:v>
+                  <c:v>1.08745</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41789</c:v>
+                  <c:v>1.0986300000000002</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41820</c:v>
+                  <c:v>1.1062000000000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41851</c:v>
+                  <c:v>1.2045899999999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41880</c:v>
+                  <c:v>1.2067399999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41912</c:v>
+                  <c:v>1.27871</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41943</c:v>
+                  <c:v>1.2983800000000001</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41971</c:v>
+                  <c:v>1.41004</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42004</c:v>
+                  <c:v>1.6953900000000002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42034</c:v>
+                  <c:v>1.7145299999999999</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42062</c:v>
+                  <c:v>1.78149</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42094</c:v>
+                  <c:v>2.0250699999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42124</c:v>
+                  <c:v>2.4119800000000002</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42153</c:v>
+                  <c:v>2.5110399999999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42185</c:v>
+                  <c:v>2.3950300000000002</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42216</c:v>
+                  <c:v>2.05552</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42247</c:v>
+                  <c:v>1.8248599999999999</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42277</c:v>
+                  <c:v>1.7126700000000001</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42307</c:v>
+                  <c:v>1.91326</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42338</c:v>
+                  <c:v>1.94798</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42369</c:v>
+                  <c:v>2.09022</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42398</c:v>
+                  <c:v>1.6191</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>42429</c:v>
+                  <c:v>1.56416</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>42460</c:v>
+                  <c:v>1.7538099999999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>42489</c:v>
+                  <c:v>1.73098</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>42521</c:v>
+                  <c:v>1.7421500000000001</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>42551</c:v>
+                  <c:v>1.75274</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>42580</c:v>
+                  <c:v>1.8355599999999999</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>42613</c:v>
+                  <c:v>1.9024799999999999</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>42643</c:v>
+                  <c:v>1.8773900000000001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>42674</c:v>
+                  <c:v>1.9152199999999999</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>42704</c:v>
+                  <c:v>2.0240299999999998</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>42734</c:v>
+                  <c:v>1.9521400000000002</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>42761</c:v>
+                  <c:v>2.0017999999999998</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>42794</c:v>
+                  <c:v>2.08507</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>42825</c:v>
+                  <c:v>2.1146199999999999</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>42853</c:v>
+                  <c:v>2.10263</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>42886</c:v>
+                  <c:v>2.0933999999999999</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>42916</c:v>
+                  <c:v>2.2407399999999997</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>42947</c:v>
+                  <c:v>2.2731599999999998</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>42978</c:v>
+                  <c:v>2.3099499999999997</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>43007</c:v>
+                  <c:v>2.33961</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>43039</c:v>
+                  <c:v>2.4434499999999999</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>43069</c:v>
+                  <c:v>2.42692</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>43098</c:v>
+                  <c:v>2.4915799999999999</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>43131</c:v>
+                  <c:v>2.6026100000000003</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>43159</c:v>
+                  <c:v>2.4634099999999997</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>43189</c:v>
+                  <c:v>2.3982399999999999</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>43217</c:v>
+                  <c:v>2.3119000000000001</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>43251</c:v>
+                  <c:v>2.3675700000000002</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>43280</c:v>
+                  <c:v>2.1851400000000001</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>43312</c:v>
+                  <c:v>2.1775900000000004</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>43343</c:v>
+                  <c:v>2.04325</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>43371</c:v>
+                  <c:v>2.10771</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>43404</c:v>
+                  <c:v>1.88317</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>43434</c:v>
+                  <c:v>1.9444000000000001</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>43462</c:v>
+                  <c:v>1.8736900000000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>43496</c:v>
+                  <c:v>1.9604600000000001</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>43524</c:v>
+                  <c:v>2.2494399999999999</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>43553</c:v>
+                  <c:v>2.4353899999999999</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>43585</c:v>
+                  <c:v>2.42089</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>43616</c:v>
+                  <c:v>2.2623000000000002</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>43644</c:v>
+                  <c:v>2.3454800000000002</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>43677</c:v>
+                  <c:v>2.3299000000000003</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>43707</c:v>
+                  <c:v>2.24383</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>43738</c:v>
+                  <c:v>2.2523499999999999</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>43769</c:v>
+                  <c:v>2.25983</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>43798</c:v>
+                  <c:v>2.2531300000000001</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>43830</c:v>
+                  <c:v>2.4450100000000003</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>43853</c:v>
+                  <c:v>2.3811999999999998</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>43889</c:v>
+                  <c:v>2.3709600000000002</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>43921</c:v>
+                  <c:v>2.1931400000000001</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>43951</c:v>
+                  <c:v>2.2996099999999999</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>43980</c:v>
+                  <c:v>2.3069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>44012</c:v>
+                  <c:v>2.4672199999999997</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>44043</c:v>
+                  <c:v>2.7463200000000003</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>44074</c:v>
+                  <c:v>2.8232600000000003</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>44104</c:v>
+                  <c:v>2.7159299999999997</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>44134</c:v>
+                  <c:v>2.8166100000000003</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>44165</c:v>
+                  <c:v>2.9742600000000001</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>44196</c:v>
+                  <c:v>3.1853200000000004</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>44225</c:v>
+                  <c:v>3.2828000000000004</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>44253</c:v>
+                  <c:v>3.2778700000000001</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>44286</c:v>
+                  <c:v>3.1244299999999998</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>44316</c:v>
+                  <c:v>3.1956700000000002</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>44347</c:v>
+                  <c:v>3.3188599999999999</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>44377</c:v>
+                  <c:v>3.2336</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>44407</c:v>
+                  <c:v>2.9186799999999997</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>44439</c:v>
+                  <c:v>2.91865</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>44469</c:v>
+                  <c:v>2.9991300000000001</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>44498</c:v>
+                  <c:v>3.0190700000000001</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>44530</c:v>
+                  <c:v>2.96435</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>44561</c:v>
+                  <c:v>3.07491</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>44589</c:v>
+                  <c:v>2.8309000000000002</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>44620</c:v>
+                  <c:v>2.8623000000000003</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>44651</c:v>
+                  <c:v>2.6462500000000002</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>44680</c:v>
+                  <c:v>2.5422700195312502</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>44712</c:v>
+                  <c:v>2.5905100097656248</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>44742</c:v>
+                  <c:v>2.8271101074218752</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>44771</c:v>
+                  <c:v>2.6160200195312502</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>44804</c:v>
+                  <c:v>2.5657299804687499</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>44834</c:v>
+                  <c:v>2.4191298828124999</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>44865</c:v>
+                  <c:v>2.1911298828125001</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>44895</c:v>
+                  <c:v>2.4362099609375001</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>44925</c:v>
+                  <c:v>2.4624399414062501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3090,448 +3089,448 @@
                 <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="148"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4270.6306042647284</c:v>
+                  <c:v>270.63060426472839</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6019.0482795100788</c:v>
+                  <c:v>19.048279510078828</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7908.6759332370966</c:v>
+                  <c:v>-91.324066762903385</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9813.8456266207759</c:v>
+                  <c:v>-186.15437337922413</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12594.595673687232</c:v>
+                  <c:v>594.59567368723219</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14359.198066862755</c:v>
+                  <c:v>359.19806686275479</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16322.087601550247</c:v>
+                  <c:v>322.0876015502472</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17451.269266820571</c:v>
+                  <c:v>-548.73073317942908</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19942.353108342035</c:v>
+                  <c:v>-57.64689165796517</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21576.949177009552</c:v>
+                  <c:v>-423.05082299044807</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22392.388248145049</c:v>
+                  <c:v>-1607.6117518549509</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22347.845830914623</c:v>
+                  <c:v>-3652.1541690853774</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25190.641898805072</c:v>
+                  <c:v>-2809.3581011949282</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25572.51743182947</c:v>
+                  <c:v>-4427.4825681705297</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25685.572979740344</c:v>
+                  <c:v>-6314.4270202596563</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28933.132851233735</c:v>
+                  <c:v>-5066.867148766265</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33381.74807603209</c:v>
+                  <c:v>-2618.2519239679095</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32987.909616819947</c:v>
+                  <c:v>-5012.0903831800533</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36761.405824874695</c:v>
+                  <c:v>-3238.5941751253049</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>40048.882763725363</c:v>
+                  <c:v>-1951.1172362746365</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39720.316947209474</c:v>
+                  <c:v>-4279.6830527905258</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39080.008691080729</c:v>
+                  <c:v>-6919.9913089192705</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>39042.86839026583</c:v>
+                  <c:v>-8957.1316097341696</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42039.486393141306</c:v>
+                  <c:v>-7960.5136068586944</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43768.754627599286</c:v>
+                  <c:v>-8231.2453724007137</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43369.954706807272</c:v>
+                  <c:v>-10630.045293192728</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>52348.707732068309</c:v>
+                  <c:v>-3651.2922679316907</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>56975.149886290856</c:v>
+                  <c:v>-1024.8501137091444</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>59626.271202087191</c:v>
+                  <c:v>-373.72879791280866</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>58909.813576350352</c:v>
+                  <c:v>-3090.1864236496476</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>60765.975625274667</c:v>
+                  <c:v>-3234.0243747253335</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>67749.102248046562</c:v>
+                  <c:v>1749.1022480465617</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>60487.473021410515</c:v>
+                  <c:v>-7512.5269785894852</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>63907.953033010097</c:v>
+                  <c:v>-6092.046966989903</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>70366.560951465755</c:v>
+                  <c:v>-1633.4390485342446</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>76555.63905651767</c:v>
+                  <c:v>2555.6390565176698</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>78788.822723998164</c:v>
+                  <c:v>2788.8227239981643</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>83307.742376054724</c:v>
+                  <c:v>5307.7423760547244</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>82813.626416639017</c:v>
+                  <c:v>2813.6264166390174</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>82019.983432432651</c:v>
+                  <c:v>19.983432432651171</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>83190.380954504973</c:v>
+                  <c:v>-809.61904549502651</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>83445.838209394322</c:v>
+                  <c:v>-2554.1617906056781</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>84569.610970805807</c:v>
+                  <c:v>-3430.3890291941934</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>87439.065429083086</c:v>
+                  <c:v>-2560.9345709169138</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>90041.555553418075</c:v>
+                  <c:v>-1958.4444465819251</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>100050.2236522255</c:v>
+                  <c:v>6050.2236522254971</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>102228.79725889026</c:v>
+                  <c:v>6228.797258890263</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>110325.72496388252</c:v>
+                  <c:v>12325.724963882516</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>114022.8314305869</c:v>
+                  <c:v>14022.831430586899</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>125828.73521648881</c:v>
+                  <c:v>23828.735216488814</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>153292.71467382699</c:v>
+                  <c:v>49292.714673826995</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>157023.30324569365</c:v>
+                  <c:v>51023.303245693649</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>165155.75959544061</c:v>
+                  <c:v>57155.759595440613</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>189737.21664670523</c:v>
+                  <c:v>79737.21664670523</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>227988.4210459491</c:v>
+                  <c:v>115988.4210459491</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>239351.90374017198</c:v>
+                  <c:v>125351.90374017198</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>230293.85036272786</c:v>
+                  <c:v>114293.85036272786</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>199648.30306826817</c:v>
+                  <c:v>81648.303068268171</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>179244.7859116719</c:v>
+                  <c:v>59244.785911671905</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>170225.05150386505</c:v>
+                  <c:v>48225.051503865048</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>192162.01722473378</c:v>
+                  <c:v>68162.017224733776</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>197649.18846023903</c:v>
+                  <c:v>71649.188460239035</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>214081.38004669495</c:v>
+                  <c:v>86081.380046694947</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>167829.03351494283</c:v>
+                  <c:v>37829.033514942828</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>164134.18631507194</c:v>
+                  <c:v>32134.186315071944</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>186034.99469442785</c:v>
+                  <c:v>52034.994694427849</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>185613.30766511807</c:v>
+                  <c:v>49613.307665118075</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>188811.06884469232</c:v>
+                  <c:v>50811.068844692316</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>191958.79390801364</c:v>
+                  <c:v>51958.793908013642</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>203029.179311132</c:v>
+                  <c:v>61029.179311132</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>212431.12350227855</c:v>
+                  <c:v>68431.123502278555</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>211629.57137627876</c:v>
+                  <c:v>65629.571376278764</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>217893.97391659516</c:v>
+                  <c:v>69893.973916595161</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>232273.25321707482</c:v>
+                  <c:v>82273.253217074816</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>226023.31414810085</c:v>
+                  <c:v>74023.31414810085</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>233773.064565896</c:v>
+                  <c:v>79773.064565895998</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>245497.45415846378</c:v>
+                  <c:v>89497.454158463777</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>250976.68975745208</c:v>
+                  <c:v>92976.689757452084</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>251553.63951192721</c:v>
+                  <c:v>91553.639511927206</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>252449.38432071661</c:v>
+                  <c:v>90449.384320716606</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>272217.55680844683</c:v>
+                  <c:v>108217.55680844683</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>278156.11870841286</c:v>
+                  <c:v>112156.11870841286</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>284657.94154854841</c:v>
+                  <c:v>116657.94154854841</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>290312.97933998541</c:v>
+                  <c:v>120312.97933998541</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>305198.0754776597</c:v>
+                  <c:v>133198.0754776597</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>305133.40290910058</c:v>
+                  <c:v>131133.40290910058</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>315263.01815480401</c:v>
+                  <c:v>139263.01815480401</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>331311.795599529</c:v>
+                  <c:v>153311.795599529</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>315591.66006348841</c:v>
+                  <c:v>135591.66006348841</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>309242.62012034556</c:v>
+                  <c:v>127242.62012034556</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>300109.45253862289</c:v>
+                  <c:v>116109.45253862289</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>309336.01650022384</c:v>
+                  <c:v>123336.01650022384</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>287500.53561047785</c:v>
+                  <c:v>99500.535610477848</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>288507.17635484249</c:v>
+                  <c:v>98507.176354842493</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>272708.57603452983</c:v>
+                  <c:v>80708.576034529833</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>283311.9259971804</c:v>
+                  <c:v>89311.925997180399</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>255129.94656765409</c:v>
+                  <c:v>59129.946567654086</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>265425.32437652821</c:v>
+                  <c:v>67425.32437652821</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>257772.87391023306</c:v>
+                  <c:v>57772.873910233058</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>271710.25537098217</c:v>
+                  <c:v>69710.255370982166</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>313761.48293854605</c:v>
+                  <c:v>109761.48293854605</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>341698.58183979383</c:v>
+                  <c:v>135698.58183979383</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>341664.15226725023</c:v>
+                  <c:v>133664.15226725023</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>321282.08703171159</c:v>
+                  <c:v>111282.08703171159</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>335094.9518150285</c:v>
+                  <c:v>123094.9518150285</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>334869.06229592022</c:v>
+                  <c:v>120869.06229592022</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>324498.4969532832</c:v>
+                  <c:v>108498.4969532832</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>327730.64341448661</c:v>
+                  <c:v>109730.64341448661</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>330819.02897301014</c:v>
+                  <c:v>110819.02897301014</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>331838.20851566637</c:v>
+                  <c:v>109838.20851566637</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>362098.05834678403</c:v>
+                  <c:v>138098.05834678403</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>354648.00411260565</c:v>
+                  <c:v>128648.00411260565</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>355122.89258811681</c:v>
+                  <c:v>127122.89258811681</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>330488.97520443297</c:v>
+                  <c:v>100488.97520443297</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>348533.16809226322</c:v>
+                  <c:v>116533.16809226322</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>351653.21023514908</c:v>
+                  <c:v>117653.21023514908</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>378075.35039287584</c:v>
+                  <c:v>142075.35039287584</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>422844.47122306196</c:v>
+                  <c:v>184844.47122306196</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>436690.74318550713</c:v>
+                  <c:v>196690.74318550713</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>422089.3612844068</c:v>
+                  <c:v>180089.3612844068</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>439736.28771259688</c:v>
+                  <c:v>195736.28771259688</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>466349.00504225586</c:v>
+                  <c:v>220349.00504225586</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>501442.15123802173</c:v>
+                  <c:v>253442.15123802173</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>518787.73061550414</c:v>
+                  <c:v>268787.73061550414</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>520008.63243348437</c:v>
+                  <c:v>268008.63243348437</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>497666.56744597905</c:v>
+                  <c:v>243666.56744597905</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>511013.84239368205</c:v>
+                  <c:v>255013.84239368205</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>532712.93374055997</c:v>
+                  <c:v>274712.93374055997</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>521027.78138983715</c:v>
+                  <c:v>261027.78138983715</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>472284.93474359531</c:v>
+                  <c:v>210284.93474359531</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>474280.08030664356</c:v>
+                  <c:v>210280.08030664356</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>489358.06528705527</c:v>
+                  <c:v>223358.06528705527</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>494611.60875526897</c:v>
+                  <c:v>226611.60875526897</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>487646.87881158153</c:v>
+                  <c:v>217646.87881158153</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>507834.42040464858</c:v>
+                  <c:v>235834.42040464858</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>469535.13459695398</c:v>
+                  <c:v>195535.13459695398</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>476743.16145284584</c:v>
+                  <c:v>200743.16145284584</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>442757.9886785429</c:v>
+                  <c:v>164757.9886785429</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>427360.55192268913</c:v>
+                  <c:v>147360.55192268913</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>437469.78842900984</c:v>
+                  <c:v>155469.78842900984</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>479425.39341558446</c:v>
+                  <c:v>195425.39341558446</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>445628.43306111766</c:v>
+                  <c:v>159628.43306111766</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>439061.72824284952</c:v>
+                  <c:v>151061.72824284952</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>415974.71880401362</c:v>
+                  <c:v>125974.71880401362</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>378769.61594403378</c:v>
+                  <c:v>86769.61594403378</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>423135.37791693263</c:v>
+                  <c:v>129135.37791693263</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>429691.15630892606</c:v>
+                  <c:v>133691.15630892606</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3573,451 +3572,451 @@
             <c:numRef>
               <c:f>'model1&amp;2'!时间</c:f>
               <c:numCache>
-                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="148"/>
                 <c:pt idx="0">
-                  <c:v>40451</c:v>
+                  <c:v>1.2300899999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40480</c:v>
+                  <c:v>1.3965399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40512</c:v>
+                  <c:v>1.31427</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40543</c:v>
+                  <c:v>1.29017</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40574</c:v>
+                  <c:v>1.2746999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40602</c:v>
+                  <c:v>1.3761099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40633</c:v>
+                  <c:v>1.3503900000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40662</c:v>
+                  <c:v>1.3469</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40694</c:v>
+                  <c:v>1.27504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40724</c:v>
+                  <c:v>1.3109200000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40753</c:v>
+                  <c:v>1.2869000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40786</c:v>
+                  <c:v>1.2162500000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40816</c:v>
+                  <c:v>1.1052</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40847</c:v>
+                  <c:v>1.1468800000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40877</c:v>
+                  <c:v>1.07321</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40907</c:v>
+                  <c:v>0.99402000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40939</c:v>
+                  <c:v>1.0423</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40968</c:v>
+                  <c:v>1.1305099999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40998</c:v>
+                  <c:v>1.0494400000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41026</c:v>
+                  <c:v>1.1058599999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41060</c:v>
+                  <c:v>1.14459</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41089</c:v>
+                  <c:v>1.0780399999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41121</c:v>
+                  <c:v>1.0063800000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41152</c:v>
+                  <c:v>0.95391999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41180</c:v>
+                  <c:v>0.97826999999999997</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41213</c:v>
+                  <c:v>0.97197</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41243</c:v>
+                  <c:v>0.91870000000000007</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41274</c:v>
+                  <c:v>1.06653</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41305</c:v>
+                  <c:v>1.1200399999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41333</c:v>
+                  <c:v>1.1328399999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41362</c:v>
+                  <c:v>1.0812299999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41390</c:v>
+                  <c:v>1.0785899999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41425</c:v>
+                  <c:v>1.1670399999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41453</c:v>
+                  <c:v>1.0075000000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41486</c:v>
+                  <c:v>1.0311600000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41516</c:v>
+                  <c:v>1.1031</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41547</c:v>
+                  <c:v>1.1687700000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41578</c:v>
+                  <c:v>1.1723299999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41607</c:v>
+                  <c:v>1.2098100000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41639</c:v>
+                  <c:v>1.1735899999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41669</c:v>
+                  <c:v>1.1339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41698</c:v>
+                  <c:v>1.12253</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41729</c:v>
+                  <c:v>1.0989899999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41759</c:v>
+                  <c:v>1.08745</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41789</c:v>
+                  <c:v>1.0986300000000002</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41820</c:v>
+                  <c:v>1.1062000000000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41851</c:v>
+                  <c:v>1.2045899999999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41880</c:v>
+                  <c:v>1.2067399999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41912</c:v>
+                  <c:v>1.27871</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41943</c:v>
+                  <c:v>1.2983800000000001</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41971</c:v>
+                  <c:v>1.41004</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42004</c:v>
+                  <c:v>1.6953900000000002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42034</c:v>
+                  <c:v>1.7145299999999999</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42062</c:v>
+                  <c:v>1.78149</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42094</c:v>
+                  <c:v>2.0250699999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42124</c:v>
+                  <c:v>2.4119800000000002</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42153</c:v>
+                  <c:v>2.5110399999999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42185</c:v>
+                  <c:v>2.3950300000000002</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42216</c:v>
+                  <c:v>2.05552</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42247</c:v>
+                  <c:v>1.8248599999999999</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42277</c:v>
+                  <c:v>1.7126700000000001</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42307</c:v>
+                  <c:v>1.91326</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42338</c:v>
+                  <c:v>1.94798</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42369</c:v>
+                  <c:v>2.09022</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42398</c:v>
+                  <c:v>1.6191</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>42429</c:v>
+                  <c:v>1.56416</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>42460</c:v>
+                  <c:v>1.7538099999999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>42489</c:v>
+                  <c:v>1.73098</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>42521</c:v>
+                  <c:v>1.7421500000000001</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>42551</c:v>
+                  <c:v>1.75274</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>42580</c:v>
+                  <c:v>1.8355599999999999</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>42613</c:v>
+                  <c:v>1.9024799999999999</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>42643</c:v>
+                  <c:v>1.8773900000000001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>42674</c:v>
+                  <c:v>1.9152199999999999</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>42704</c:v>
+                  <c:v>2.0240299999999998</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>42734</c:v>
+                  <c:v>1.9521400000000002</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>42761</c:v>
+                  <c:v>2.0017999999999998</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>42794</c:v>
+                  <c:v>2.08507</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>42825</c:v>
+                  <c:v>2.1146199999999999</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>42853</c:v>
+                  <c:v>2.10263</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>42886</c:v>
+                  <c:v>2.0933999999999999</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>42916</c:v>
+                  <c:v>2.2407399999999997</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>42947</c:v>
+                  <c:v>2.2731599999999998</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>42978</c:v>
+                  <c:v>2.3099499999999997</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>43007</c:v>
+                  <c:v>2.33961</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>43039</c:v>
+                  <c:v>2.4434499999999999</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>43069</c:v>
+                  <c:v>2.42692</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>43098</c:v>
+                  <c:v>2.4915799999999999</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>43131</c:v>
+                  <c:v>2.6026100000000003</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>43159</c:v>
+                  <c:v>2.4634099999999997</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>43189</c:v>
+                  <c:v>2.3982399999999999</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>43217</c:v>
+                  <c:v>2.3119000000000001</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>43251</c:v>
+                  <c:v>2.3675700000000002</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>43280</c:v>
+                  <c:v>2.1851400000000001</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>43312</c:v>
+                  <c:v>2.1775900000000004</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>43343</c:v>
+                  <c:v>2.04325</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>43371</c:v>
+                  <c:v>2.10771</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>43404</c:v>
+                  <c:v>1.88317</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>43434</c:v>
+                  <c:v>1.9444000000000001</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>43462</c:v>
+                  <c:v>1.8736900000000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>43496</c:v>
+                  <c:v>1.9604600000000001</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>43524</c:v>
+                  <c:v>2.2494399999999999</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>43553</c:v>
+                  <c:v>2.4353899999999999</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>43585</c:v>
+                  <c:v>2.42089</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>43616</c:v>
+                  <c:v>2.2623000000000002</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>43644</c:v>
+                  <c:v>2.3454800000000002</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>43677</c:v>
+                  <c:v>2.3299000000000003</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>43707</c:v>
+                  <c:v>2.24383</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>43738</c:v>
+                  <c:v>2.2523499999999999</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>43769</c:v>
+                  <c:v>2.25983</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>43798</c:v>
+                  <c:v>2.2531300000000001</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>43830</c:v>
+                  <c:v>2.4450100000000003</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>43853</c:v>
+                  <c:v>2.3811999999999998</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>43889</c:v>
+                  <c:v>2.3709600000000002</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>43921</c:v>
+                  <c:v>2.1931400000000001</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>43951</c:v>
+                  <c:v>2.2996099999999999</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>43980</c:v>
+                  <c:v>2.3069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>44012</c:v>
+                  <c:v>2.4672199999999997</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>44043</c:v>
+                  <c:v>2.7463200000000003</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>44074</c:v>
+                  <c:v>2.8232600000000003</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>44104</c:v>
+                  <c:v>2.7159299999999997</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>44134</c:v>
+                  <c:v>2.8166100000000003</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>44165</c:v>
+                  <c:v>2.9742600000000001</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>44196</c:v>
+                  <c:v>3.1853200000000004</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>44225</c:v>
+                  <c:v>3.2828000000000004</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>44253</c:v>
+                  <c:v>3.2778700000000001</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>44286</c:v>
+                  <c:v>3.1244299999999998</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>44316</c:v>
+                  <c:v>3.1956700000000002</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>44347</c:v>
+                  <c:v>3.3188599999999999</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>44377</c:v>
+                  <c:v>3.2336</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>44407</c:v>
+                  <c:v>2.9186799999999997</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>44439</c:v>
+                  <c:v>2.91865</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>44469</c:v>
+                  <c:v>2.9991300000000001</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>44498</c:v>
+                  <c:v>3.0190700000000001</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>44530</c:v>
+                  <c:v>2.96435</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>44561</c:v>
+                  <c:v>3.07491</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>44589</c:v>
+                  <c:v>2.8309000000000002</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>44620</c:v>
+                  <c:v>2.8623000000000003</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>44651</c:v>
+                  <c:v>2.6462500000000002</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>44680</c:v>
+                  <c:v>2.5422700195312502</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>44712</c:v>
+                  <c:v>2.5905100097656248</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>44742</c:v>
+                  <c:v>2.8271101074218752</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>44771</c:v>
+                  <c:v>2.6160200195312502</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>44804</c:v>
+                  <c:v>2.5657299804687499</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>44834</c:v>
+                  <c:v>2.4191298828124999</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>44865</c:v>
+                  <c:v>2.1911298828125001</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>44895</c:v>
+                  <c:v>2.4362099609375001</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>44925</c:v>
+                  <c:v>2.4624399414062501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4026,451 +4025,451 @@
             <c:numRef>
               <c:f>'model1&amp;2'!金额</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="148"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>270.63060426472839</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.048279510078828</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-91.324066762903385</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-186.15437337922413</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>594.59567368723219</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>359.19806686275479</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>322.0876015502472</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-548.73073317942908</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-57.64689165796517</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-423.05082299044807</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1607.6117518549509</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-3652.1541690853774</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2809.3581011949282</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4427.4825681705297</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-6314.4270202596563</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-5066.867148766265</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2618.2519239679095</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-5012.0903831800533</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-3238.5941751253049</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1951.1172362746365</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-4279.6830527905258</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-6919.9913089192705</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-8957.1316097341696</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-7960.5136068586944</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-8231.2453724007137</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-10630.045293192728</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-3651.2922679316907</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-1024.8501137091444</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-373.72879791280866</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-3090.1864236496476</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-3234.0243747253335</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1749.1022480465617</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-7512.5269785894852</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-6092.046966989903</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1633.4390485342446</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2555.6390565176698</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2788.8227239981643</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5307.7423760547244</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2813.6264166390174</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>19.983432432651171</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-809.61904549502651</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-2554.1617906056781</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-3430.3890291941934</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-2560.9345709169138</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-1958.4444465819251</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6050.2236522254971</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6228.797258890263</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>12325.724963882516</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>14022.831430586899</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>23828.735216488814</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>49292.714673826995</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>51023.303245693649</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>57155.759595440613</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>79737.21664670523</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>115988.4210459491</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>125351.90374017198</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>114293.85036272786</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>81648.303068268171</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>59244.785911671905</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>48225.051503865048</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>68162.017224733776</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>71649.188460239035</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>86081.380046694947</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>37829.033514942828</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>32134.186315071944</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>52034.994694427849</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>49613.307665118075</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>50811.068844692316</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>51958.793908013642</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>61029.179311132</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>68431.123502278555</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>65629.571376278764</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>69893.973916595161</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>82273.253217074816</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>74023.31414810085</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>79773.064565895998</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>89497.454158463777</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>92976.689757452084</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>91553.639511927206</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>90449.384320716606</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>108217.55680844683</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>112156.11870841286</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>116657.94154854841</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>120312.97933998541</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>133198.0754776597</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>131133.40290910058</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>139263.01815480401</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>153311.795599529</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>135591.66006348841</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>127242.62012034556</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>116109.45253862289</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>123336.01650022384</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>99500.535610477848</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>98507.176354842493</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>80708.576034529833</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>89311.925997180399</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>59129.946567654086</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>67425.32437652821</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>57772.873910233058</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>69710.255370982166</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>109761.48293854605</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>135698.58183979383</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>133664.15226725023</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>111282.08703171159</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>123094.9518150285</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>120869.06229592022</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>108498.4969532832</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>109730.64341448661</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>110819.02897301014</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>109838.20851566637</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>138098.05834678403</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>128648.00411260565</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>127122.89258811681</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>100488.97520443297</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>116533.16809226322</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>117653.21023514908</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>142075.35039287584</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>184844.47122306196</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>196690.74318550713</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>180089.3612844068</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>195736.28771259688</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>220349.00504225586</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>253442.15123802173</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>268787.73061550414</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>268008.63243348437</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>243666.56744597905</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>255013.84239368205</c:v>
+                  <c:v>16.649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>274712.93374055997</c:v>
+                  <c:v>14.94</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>261027.78138983715</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>210284.93474359531</c:v>
+                  <c:v>13.310000419616699</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>210280.08030664356</c:v>
+                  <c:v>13.430000305175781</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>223358.06528705527</c:v>
+                  <c:v>12.899999618530273</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>226611.60875526897</c:v>
+                  <c:v>12.840000152587891</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>217646.87881158153</c:v>
+                  <c:v>12.390000343322754</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>235834.42040464858</c:v>
+                  <c:v>12.949999809265137</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>195535.13459695398</c:v>
+                  <c:v>12.039999961853027</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>200743.16145284584</c:v>
+                  <c:v>12.239999771118164</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>164757.9886785429</c:v>
+                  <c:v>11.460000040000001</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>147360.55192268913</c:v>
+                  <c:v>11.14000034</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>155469.78842900984</c:v>
+                  <c:v>10.93999958</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>195425.39341558446</c:v>
+                  <c:v>12.100000380000001</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>159628.43306111766</c:v>
+                  <c:v>11.239999770000001</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>151061.72824284952</c:v>
+                  <c:v>11.100000380000001</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>125974.71880401362</c:v>
+                  <c:v>10.3500003814697</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>86769.61594403378</c:v>
+                  <c:v>9.3900003430000005</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>129135.37791693263</c:v>
+                  <c:v>10.380000109999999</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>133691.15630892606</c:v>
+                  <c:v>10.72999954</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4492,17 +4491,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="77947264"/>
-        <c:axId val="77948800"/>
+        <c:axId val="558619264"/>
+        <c:axId val="560267648"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="77947264"/>
+      <c:catAx>
+        <c:axId val="558619264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -4539,14 +4538,15 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77948800"/>
+        <c:crossAx val="560267648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="77948800"/>
+        <c:axId val="560267648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4597,7 +4597,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77947264"/>
+        <c:crossAx val="558619264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4611,7 +4611,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -64443,7 +64442,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -71783,7 +71782,7 @@
       </c>
       <c r="J147" s="31">
         <f>VLOOKUP(A147,myPEPB!B:C,2)</f>
-        <v>10.100000380000001</v>
+        <v>10.3500003814697</v>
       </c>
     </row>
     <row r="148" spans="1:10" ht="12.75">
@@ -71924,7 +71923,7 @@
   </sheetPr>
   <dimension ref="A1:D424"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -77417,11 +77416,11 @@
         <v>195</v>
       </c>
       <c r="C344" s="21">
-        <v>10.55</v>
+        <v>10.77999973</v>
       </c>
       <c r="D344" s="17">
         <f>SUM($C$3:C344)/A344</f>
-        <v>12.74526316497885</v>
+        <v>12.745935678809259</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="12.75" customHeight="1">
@@ -77433,11 +77432,11 @@
         <v>196</v>
       </c>
       <c r="C345" s="21">
-        <v>10.55000019</v>
+        <v>10.7211</v>
       </c>
       <c r="D345" s="17">
         <f>SUM($C$3:C345)/A345</f>
-        <v>12.738862981378329</v>
+        <v>12.74003236779232</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="12.75" customHeight="1">
@@ -77449,11 +77448,11 @@
         <v>197</v>
       </c>
       <c r="C346" s="21">
-        <v>10.55</v>
+        <v>10.72999954</v>
       </c>
       <c r="D346" s="17">
         <f>SUM($C$3:C346)/A346</f>
-        <v>12.732500007595252</v>
+        <v>12.734189249106878</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="12.75" customHeight="1">
@@ -77465,11 +77464,11 @@
         <v>198</v>
       </c>
       <c r="C347" s="21">
-        <v>10.49</v>
+        <v>10.81999969</v>
       </c>
       <c r="D347" s="17">
         <f>SUM($C$3:C347)/A347</f>
-        <v>12.726000007573237</v>
+        <v>12.728640873573235</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="12.75" customHeight="1">
@@ -77481,11 +77480,11 @@
         <v>199</v>
       </c>
       <c r="C348" s="21">
-        <v>10.42</v>
+        <v>10.80000019</v>
       </c>
       <c r="D348" s="17">
         <f>SUM($C$3:C348)/A348</f>
-        <v>12.719335267666956</v>
+        <v>12.723066767551348</v>
       </c>
     </row>
     <row r="349" spans="1:4" ht="12.75" customHeight="1">
@@ -77497,11 +77496,11 @@
         <v>200</v>
       </c>
       <c r="C349" s="21">
-        <v>10.4</v>
+        <v>10.760000229999999</v>
       </c>
       <c r="D349" s="17">
         <f>SUM($C$3:C349)/A349</f>
-        <v>12.712651304359557</v>
+        <v>12.717409515281746</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="12.75" customHeight="1">
@@ -77513,11 +77512,11 @@
         <v>201</v>
       </c>
       <c r="C350" s="21">
-        <v>10.34</v>
+        <v>10.9177</v>
       </c>
       <c r="D350" s="17">
         <f>SUM($C$3:C350)/A350</f>
-        <v>12.705833340841282</v>
+        <v>12.712237936214844</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="12.75" customHeight="1">
@@ -77529,11 +77528,11 @@
         <v>202</v>
       </c>
       <c r="C351" s="21">
-        <v>10.48</v>
+        <v>10.96</v>
       </c>
       <c r="D351" s="17">
         <f>SUM($C$3:C351)/A351</f>
-        <v>12.699455594878986</v>
+        <v>12.707217197142596</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="12.75" customHeight="1">
@@ -77545,11 +77544,11 @@
         <v>203</v>
       </c>
       <c r="C352" s="21">
-        <v>10.37</v>
+        <v>10.85</v>
       </c>
       <c r="D352" s="17">
         <f>SUM($C$3:C352)/A352</f>
-        <v>12.692800007465046</v>
+        <v>12.701910862293618</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="12.75" customHeight="1">
@@ -77561,11 +77560,11 @@
         <v>204</v>
       </c>
       <c r="C353" s="21">
-        <v>10.37</v>
+        <v>10.78</v>
       </c>
       <c r="D353" s="17">
         <f>SUM($C$3:C353)/A353</f>
-        <v>12.686182343626113</v>
+        <v>12.696435332771413</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="12.75" customHeight="1">
@@ -77577,11 +77576,11 @@
         <v>205</v>
       </c>
       <c r="C354" s="21">
-        <v>10.350000380000001</v>
+        <v>10.55</v>
       </c>
       <c r="D354" s="17">
         <f>SUM($C$3:C354)/A354</f>
-        <v>12.67954546304763</v>
+        <v>12.690337505121494</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="12.75" customHeight="1">
@@ -77593,11 +77592,11 @@
         <v>206</v>
       </c>
       <c r="C355" s="21">
-        <v>10.149999619999999</v>
+        <v>10.55000019</v>
       </c>
       <c r="D355" s="17">
         <f>SUM($C$3:C355)/A355</f>
-        <v>12.672379610801036</v>
+        <v>12.684274226608403</v>
       </c>
     </row>
     <row r="356" spans="1:4" ht="12.75" customHeight="1">
@@ -77609,11 +77608,11 @@
         <v>207</v>
       </c>
       <c r="C356" s="21">
-        <v>10.15999985</v>
+        <v>10.55</v>
       </c>
       <c r="D356" s="17">
         <f>SUM($C$3:C356)/A356</f>
-        <v>12.66528249283267</v>
+        <v>12.678245203369396</v>
       </c>
     </row>
     <row r="357" spans="1:4" ht="12.75" customHeight="1">
@@ -77625,11 +77624,11 @@
         <v>208</v>
       </c>
       <c r="C357" s="21">
-        <v>10.260000229999999</v>
+        <v>10.49</v>
       </c>
       <c r="D357" s="17">
         <f>SUM($C$3:C357)/A357</f>
-        <v>12.658507049838775</v>
+        <v>12.672081132373989</v>
       </c>
     </row>
     <row r="358" spans="1:4" ht="12.75" customHeight="1">
@@ -77641,11 +77640,11 @@
         <v>209</v>
       </c>
       <c r="C358" s="21">
-        <v>10.170000079999999</v>
+        <v>10.42</v>
       </c>
       <c r="D358" s="17">
         <f>SUM($C$3:C358)/A358</f>
-        <v>12.65151686172125</v>
+        <v>12.665755061777434</v>
       </c>
     </row>
     <row r="359" spans="1:4" ht="12.75" customHeight="1">
@@ -77657,11 +77656,11 @@
         <v>210</v>
       </c>
       <c r="C359" s="21">
-        <v>10.39000034</v>
+        <v>10.4</v>
       </c>
       <c r="D359" s="17">
         <f>SUM($C$3:C359)/A359</f>
-        <v>12.645182081548363</v>
+        <v>12.659408408943321</v>
       </c>
     </row>
     <row r="360" spans="1:4" ht="12.75" customHeight="1">
@@ -77673,11 +77672,11 @@
         <v>211</v>
       </c>
       <c r="C360" s="21">
-        <v>10.369999890000001</v>
+        <v>10.34</v>
       </c>
       <c r="D360" s="17">
         <f>SUM($C$3:C360)/A360</f>
-        <v>12.638826824030073</v>
+        <v>12.652929614504933</v>
       </c>
     </row>
     <row r="361" spans="1:4" ht="12.75" customHeight="1">
@@ -77689,11 +77688,11 @@
         <v>212</v>
       </c>
       <c r="C361" s="21">
-        <v>10.350000380000001</v>
+        <v>10.48</v>
       </c>
       <c r="D361" s="17">
         <f>SUM($C$3:C361)/A361</f>
-        <v>12.63245126290464</v>
+        <v>12.64687688577372</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="12.75" customHeight="1">
@@ -77705,11 +77704,11 @@
         <v>213</v>
       </c>
       <c r="C362" s="21">
-        <v>10.18000031</v>
+        <v>10.37</v>
       </c>
       <c r="D362" s="17">
         <f>SUM($C$3:C362)/A362</f>
-        <v>12.625638899146571</v>
+        <v>12.640552227757683</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="12.75" customHeight="1">
@@ -77721,11 +77720,11 @@
         <v>214</v>
       </c>
       <c r="C363" s="21">
-        <v>10.119999890000001</v>
+        <v>10.369999890000001</v>
       </c>
       <c r="D363" s="17">
         <f>SUM($C$3:C363)/A363</f>
-        <v>12.618698070866387</v>
+        <v>12.634262609093533</v>
       </c>
     </row>
     <row r="364" spans="1:4" ht="12.75" customHeight="1">
@@ -77737,11 +77736,11 @@
         <v>44834</v>
       </c>
       <c r="C364" s="21">
-        <v>10.100000380000001</v>
+        <v>10.3500003814697</v>
       </c>
       <c r="D364" s="17">
         <f>SUM($C$3:C364)/A364</f>
-        <v>12.611740342438578</v>
+        <v>12.627952492442638</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="12.75" customHeight="1">
@@ -77757,7 +77756,7 @@
       </c>
       <c r="D365" s="17">
         <f>SUM($C$3:C365)/A365</f>
-        <v>12.604958687555827</v>
+        <v>12.621126175989628</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="12.75" customHeight="1">
@@ -77773,7 +77772,7 @@
       </c>
       <c r="D366" s="17">
         <f>SUM($C$3:C366)/A366</f>
-        <v>12.598241767672432</v>
+        <v>12.614364839929216</v>
       </c>
     </row>
     <row r="367" spans="1:4" ht="12.75" customHeight="1">
@@ -77789,7 +77788,7 @@
       </c>
       <c r="D367" s="17">
         <f>SUM($C$3:C367)/A367</f>
-        <v>12.591835626473328</v>
+        <v>12.607914525929409</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="12.75" customHeight="1">
@@ -77805,7 +77804,7 @@
       </c>
       <c r="D368" s="17">
         <f>SUM($C$3:C368)/A368</f>
-        <v>12.585218589461107</v>
+        <v>12.601253557497909</v>
       </c>
     </row>
     <row r="369" spans="1:4" ht="12.75" customHeight="1">
@@ -77821,7 +77820,7 @@
       </c>
       <c r="D369" s="17">
         <f>SUM($C$3:C369)/A369</f>
-        <v>12.57923706834541</v>
+        <v>12.595228344371213</v>
       </c>
     </row>
     <row r="370" spans="1:4" ht="12.75" customHeight="1">
@@ -77837,7 +77836,7 @@
       </c>
       <c r="D370" s="17">
         <f>SUM($C$3:C370)/A370</f>
-        <v>12.573233706447732</v>
+        <v>12.589181527919118</v>
       </c>
     </row>
     <row r="371" spans="1:4" ht="12.75" customHeight="1">
@@ -77853,7 +77852,7 @@
       </c>
       <c r="D371" s="17">
         <f>SUM($C$3:C371)/A371</f>
-        <v>12.567208683882834</v>
+        <v>12.58311328632584</v>
       </c>
     </row>
     <row r="372" spans="1:4" ht="12.75" customHeight="1">
@@ -77869,7 +77868,7 @@
       </c>
       <c r="D372" s="17">
         <f>SUM($C$3:C372)/A372</f>
-        <v>12.560756769358825</v>
+        <v>12.576618386389825</v>
       </c>
     </row>
     <row r="373" spans="1:4" ht="12.75" customHeight="1">
@@ -77885,7 +77884,7 @@
       </c>
       <c r="D373" s="17">
         <f>SUM($C$3:C373)/A373</f>
-        <v>12.554177909845729</v>
+        <v>12.569996773192008</v>
       </c>
     </row>
     <row r="374" spans="1:4" ht="12.75" customHeight="1">
@@ -77901,7 +77900,7 @@
       </c>
       <c r="D374" s="17">
         <f>SUM($C$3:C374)/A374</f>
-        <v>12.547580658421412</v>
+        <v>12.563356997941492</v>
       </c>
     </row>
     <row r="375" spans="1:4" ht="12.75" customHeight="1">
@@ -77917,7 +77916,7 @@
       </c>
       <c r="D375" s="17">
         <f>SUM($C$3:C375)/A375</f>
-        <v>12.540241301213847</v>
+        <v>12.555975344917519</v>
       </c>
     </row>
     <row r="376" spans="1:4" ht="12.75" customHeight="1">
@@ -77933,7 +77932,7 @@
       </c>
       <c r="D376" s="17">
         <f>SUM($C$3:C376)/A376</f>
-        <v>12.532860976165148</v>
+        <v>12.548552950233248</v>
       </c>
     </row>
     <row r="377" spans="1:4" ht="12.75" customHeight="1">
@@ -77949,7 +77948,7 @@
       </c>
       <c r="D377" s="17">
         <f>SUM($C$3:C377)/A377</f>
-        <v>12.525653346692707</v>
+        <v>12.541303475496626</v>
       </c>
     </row>
     <row r="378" spans="1:4" ht="12.75" customHeight="1">
@@ -77965,7 +77964,7 @@
       </c>
       <c r="D378" s="17">
         <f>SUM($C$3:C378)/A378</f>
-        <v>12.518244693565864</v>
+        <v>12.533853199686794</v>
       </c>
     </row>
     <row r="379" spans="1:4" ht="12.75" customHeight="1">
@@ -77981,7 +77980,7 @@
       </c>
       <c r="D379" s="17">
         <f>SUM($C$3:C379)/A379</f>
-        <v>12.51031831436012</v>
+        <v>12.52588541860805</v>
       </c>
     </row>
     <row r="380" spans="1:4" ht="12.75" customHeight="1">
@@ -77997,7 +77996,7 @@
       </c>
       <c r="D380" s="17">
         <f>SUM($C$3:C380)/A380</f>
-        <v>12.502063504912076</v>
+        <v>12.517589426344536</v>
       </c>
     </row>
     <row r="381" spans="1:4" ht="12.75" customHeight="1">
@@ -78013,7 +78012,7 @@
       </c>
       <c r="D381" s="17">
         <f>SUM($C$3:C381)/A381</f>
-        <v>12.494696582835791</v>
+        <v>12.510181538776344</v>
       </c>
     </row>
     <row r="382" spans="1:4" ht="12.75" customHeight="1">
@@ -78029,7 +78028,7 @@
       </c>
       <c r="D382" s="17">
         <f>SUM($C$3:C382)/A382</f>
-        <v>12.487631592933591</v>
+        <v>12.503075798990089</v>
       </c>
     </row>
     <row r="383" spans="1:4" ht="12.75" customHeight="1">
@@ -78045,7 +78044,7 @@
       </c>
       <c r="D383" s="17">
         <f>SUM($C$3:C383)/A383</f>
-        <v>12.480419960855023</v>
+        <v>12.495823630937622</v>
       </c>
     </row>
     <row r="384" spans="1:4" ht="12.75" customHeight="1">
@@ -78061,7 +78060,7 @@
       </c>
       <c r="D384" s="17">
         <f>SUM($C$3:C384)/A384</f>
-        <v>12.473979072109332</v>
+        <v>12.489342418448256</v>
       </c>
     </row>
     <row r="385" spans="1:4" ht="12.75" customHeight="1">
@@ -78077,7 +78076,7 @@
       </c>
       <c r="D385" s="17">
         <f>SUM($C$3:C385)/A385</f>
-        <v>12.467676255785285</v>
+        <v>12.482999488948391</v>
       </c>
     </row>
     <row r="386" spans="1:4" ht="12.75" customHeight="1">
@@ -78093,7 +78092,7 @@
       </c>
       <c r="D386" s="17">
         <f>SUM($C$3:C386)/A386</f>
-        <v>12.461223973272823</v>
+        <v>12.476507302182901</v>
       </c>
     </row>
     <row r="387" spans="1:4" ht="12.75" customHeight="1">
@@ -78109,7 +78108,7 @@
       </c>
       <c r="D387" s="17">
         <f>SUM($C$3:C387)/A387</f>
-        <v>12.454623391721466</v>
+        <v>12.469867023673334</v>
       </c>
     </row>
     <row r="388" spans="1:4" ht="12.75" customHeight="1">
@@ -78125,7 +78124,7 @@
       </c>
       <c r="D388" s="17">
         <f>SUM($C$3:C388)/A388</f>
-        <v>12.447953383229958</v>
+        <v>12.463157523907341</v>
       </c>
     </row>
     <row r="389" spans="1:4" ht="12.75" customHeight="1">
@@ -78141,7 +78140,7 @@
       </c>
       <c r="D389" s="17">
         <f>SUM($C$3:C389)/A389</f>
-        <v>12.441963839888279</v>
+        <v>12.457128693380449</v>
       </c>
     </row>
     <row r="390" spans="1:4" ht="12.75" customHeight="1">
@@ -78157,7 +78156,7 @@
       </c>
       <c r="D390" s="17">
         <f>SUM($C$3:C390)/A390</f>
-        <v>12.436082489398874</v>
+        <v>12.451208258217095</v>
       </c>
     </row>
     <row r="391" spans="1:4" ht="12.75" customHeight="1">
@@ -78173,7 +78172,7 @@
       </c>
       <c r="D391" s="17">
         <f>SUM($C$3:C391)/A391</f>
-        <v>12.430616982793735</v>
+        <v>12.445703867887488</v>
       </c>
     </row>
     <row r="392" spans="1:4" ht="12.75" customHeight="1">
@@ -78189,7 +78188,7 @@
       </c>
       <c r="D392" s="17">
         <f>SUM($C$3:C392)/A392</f>
-        <v>12.425051298812212</v>
+        <v>12.440099499585211</v>
       </c>
     </row>
     <row r="393" spans="1:4" ht="12.75" customHeight="1">
@@ -78205,7 +78204,7 @@
       </c>
       <c r="D393" s="17">
         <f>SUM($C$3:C393)/A393</f>
-        <v>12.41936063004287</v>
+        <v>12.434370344368881</v>
       </c>
     </row>
     <row r="394" spans="1:4" ht="12.75" customHeight="1">
@@ -78221,7 +78220,7 @@
       </c>
       <c r="D394" s="17">
         <f>SUM($C$3:C394)/A394</f>
-        <v>12.413673484507049</v>
+        <v>12.428644908745492</v>
       </c>
     </row>
     <row r="395" spans="1:4" ht="12.75" customHeight="1">
@@ -78237,7 +78236,7 @@
       </c>
       <c r="D395" s="17">
         <f>SUM($C$3:C395)/A395</f>
-        <v>12.40783716492815</v>
+        <v>12.422770493939524</v>
       </c>
     </row>
     <row r="396" spans="1:4" ht="12.75" customHeight="1">
@@ -78253,7 +78252,7 @@
       </c>
       <c r="D396" s="17">
         <f>SUM($C$3:C396)/A396</f>
-        <v>12.402055852605997</v>
+        <v>12.416951279767089</v>
       </c>
     </row>
     <row r="397" spans="1:4" ht="12.75" customHeight="1">
@@ -78269,7 +78268,7 @@
       </c>
       <c r="D397" s="17">
         <f>SUM($C$3:C397)/A397</f>
-        <v>12.396405078498134</v>
+        <v>12.411262795717045</v>
       </c>
     </row>
     <row r="398" spans="1:4" ht="12.75" customHeight="1">
@@ -78285,7 +78284,7 @@
       </c>
       <c r="D398" s="17">
         <f>SUM($C$3:C398)/A398</f>
-        <v>12.390681833628189</v>
+        <v>12.405502031359173</v>
       </c>
     </row>
     <row r="399" spans="1:4" ht="12.75" customHeight="1">
@@ -78301,7 +78300,7 @@
       </c>
       <c r="D399" s="17">
         <f>SUM($C$3:C399)/A399</f>
-        <v>12.385163742888572</v>
+        <v>12.399946610146682</v>
       </c>
     </row>
     <row r="400" spans="1:4" ht="12.75" customHeight="1">
@@ -78317,7 +78316,7 @@
       </c>
       <c r="D400" s="17">
         <f>SUM($C$3:C400)/A400</f>
-        <v>12.379422126398902</v>
+        <v>12.394167850774455</v>
       </c>
     </row>
     <row r="401" spans="1:4" ht="12.75" customHeight="1">
@@ -78333,7 +78332,7 @@
       </c>
       <c r="D401" s="17">
         <f>SUM($C$3:C401)/A401</f>
-        <v>12.374436106884119</v>
+        <v>12.389144874556974</v>
       </c>
     </row>
     <row r="402" spans="1:4" ht="12.75" customHeight="1">
@@ -78349,7 +78348,7 @@
       </c>
       <c r="D402" s="17">
         <f>SUM($C$3:C402)/A402</f>
-        <v>12.369450016891909</v>
+        <v>12.384122012645582</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -78365,7 +78364,7 @@
       </c>
       <c r="D403" s="17">
         <f>SUM($C$3:C403)/A403</f>
-        <v>12.364713234480707</v>
+        <v>12.379348641716293</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -78381,7 +78380,7 @@
       </c>
       <c r="D404" s="17">
         <f>SUM($C$3:C404)/A404</f>
-        <v>12.359875639569063</v>
+        <v>12.374474640318988</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -78397,7 +78396,7 @@
       </c>
       <c r="D405" s="17">
         <f>SUM($C$3:C405)/A405</f>
-        <v>12.355533515550281</v>
+        <v>12.370096290491892</v>
       </c>
     </row>
     <row r="406" spans="1:4">
@@ -78413,7 +78412,7 @@
       </c>
       <c r="D406" s="17">
         <f>SUM($C$3:C406)/A406</f>
-        <v>12.351386156130602</v>
+        <v>12.365912884599586</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -78429,7 +78428,7 @@
       </c>
       <c r="D407" s="17">
         <f>SUM($C$3:C407)/A407</f>
-        <v>12.347185201720402</v>
+        <v>12.361676061724031</v>
       </c>
     </row>
     <row r="408" spans="1:4">
@@ -78445,7 +78444,7 @@
       </c>
       <c r="D408" s="17">
         <f>SUM($C$3:C408)/A408</f>
-        <v>12.343029572775277</v>
+        <v>12.357484741005498</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -78461,7 +78460,7 @@
       </c>
       <c r="D409" s="17">
         <f>SUM($C$3:C409)/A409</f>
-        <v>12.339164636380252</v>
+        <v>12.353584288226616</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -78477,7 +78476,7 @@
       </c>
       <c r="D410" s="17">
         <f>SUM($C$3:C410)/A410</f>
-        <v>12.33568629187932</v>
+        <v>12.350070601441747</v>
       </c>
     </row>
     <row r="411" spans="1:4">
@@ -78493,7 +78492,7 @@
       </c>
       <c r="D411" s="17">
         <f>SUM($C$3:C411)/A411</f>
-        <v>12.332200505957854</v>
+        <v>12.346549646059247</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -78509,7 +78508,7 @@
       </c>
       <c r="D412" s="17">
         <f>SUM($C$3:C412)/A412</f>
-        <v>12.328804893943325</v>
+        <v>12.343119036142031</v>
       </c>
     </row>
     <row r="413" spans="1:4">
@@ -78525,7 +78524,7 @@
       </c>
       <c r="D413" s="17">
         <f>SUM($C$3:C413)/A413</f>
-        <v>12.325352813544434</v>
+        <v>12.339632128146549</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -78541,7 +78540,7 @@
       </c>
       <c r="D414" s="17">
         <f>SUM($C$3:C414)/A414</f>
-        <v>12.322014578098939</v>
+        <v>12.336259234170466</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -78557,7 +78556,7 @@
       </c>
       <c r="D415" s="17">
         <f>SUM($C$3:C415)/A415</f>
-        <v>12.31828088597279</v>
+        <v>12.332491051351651</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -78573,7 +78572,7 @@
       </c>
       <c r="D416" s="17">
         <f>SUM($C$3:C416)/A416</f>
-        <v>12.314130449968024</v>
+        <v>12.328306291275922</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -78589,7 +78588,7 @@
       </c>
       <c r="D417" s="17">
         <f>SUM($C$3:C417)/A417</f>
-        <v>12.310024110715089</v>
+        <v>12.324165793369232</v>
       </c>
     </row>
     <row r="418" spans="1:4">
@@ -78605,7 +78604,7 @@
       </c>
       <c r="D418" s="17">
         <f>SUM($C$3:C418)/A418</f>
-        <v>12.306009630497025</v>
+        <v>12.320117318721712</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -78621,7 +78620,7 @@
       </c>
       <c r="D419" s="17">
         <f>SUM($C$3:C419)/A419</f>
-        <v>12.301990423013818</v>
+        <v>12.316064279851874</v>
       </c>
     </row>
     <row r="420" spans="1:4">
@@ -78637,7 +78636,7 @@
       </c>
       <c r="D420" s="17">
         <f>SUM($C$3:C420)/A420</f>
-        <v>12.297990446188425</v>
+        <v>12.312030633512515</v>
       </c>
     </row>
     <row r="421" spans="1:4">
@@ -78653,7 +78652,7 @@
       </c>
       <c r="D421" s="17">
         <f>SUM($C$3:C421)/A421</f>
-        <v>12.294295958250029</v>
+        <v>12.308302636773822</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -78669,7 +78668,7 @@
       </c>
       <c r="D422" s="17">
         <f>SUM($C$3:C422)/A422</f>
-        <v>12.290595253039911</v>
+        <v>12.304568582329123</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -78685,7 +78684,7 @@
       </c>
       <c r="D423" s="17">
         <f>SUM($C$3:C423)/A423</f>
-        <v>12.28676961184504</v>
+        <v>12.300709750328341</v>
       </c>
     </row>
     <row r="424" spans="1:4">
@@ -78701,7 +78700,7 @@
       </c>
       <c r="D424" s="17">
         <f>SUM($C$3:C424)/A424</f>
-        <v>12.283080583238773</v>
+        <v>12.296987688218559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>